<commit_message>
v0.0.16.12 xlsx 10 safe
</commit_message>
<xml_diff>
--- a/path_to_temp_xlsx.xlsx
+++ b/path_to_temp_xlsx.xlsx
@@ -948,81 +948,6 @@
         <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>37</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1764792" cy="1335024"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>37</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1764792" cy="1335024"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>49</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1764792" cy="1335024"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -2947,11 +2872,7 @@
       </c>
     </row>
     <row r="33" ht="17.45" customHeight="1" s="56">
-      <c r="A33" s="55" t="inlineStr">
-        <is>
-          <t>dfgdsfg</t>
-        </is>
-      </c>
+      <c r="A33" s="55" t="inlineStr"/>
       <c r="B33" s="107" t="n"/>
       <c r="C33" s="100" t="n"/>
       <c r="E33" s="55" t="inlineStr"/>
@@ -2959,11 +2880,7 @@
       <c r="G33" s="100" t="n"/>
     </row>
     <row r="34" ht="17.45" customHeight="1" s="56">
-      <c r="A34" s="78" t="inlineStr">
-        <is>
-          <t>sdfg</t>
-        </is>
-      </c>
+      <c r="A34" s="78" t="inlineStr"/>
       <c r="B34" s="107" t="n"/>
       <c r="C34" s="100" t="n"/>
       <c r="E34" s="78" t="inlineStr"/>

</xml_diff>